<commit_message>
Change color PK and bold FK
</commit_message>
<xml_diff>
--- a/DB_Design.xlsx
+++ b/DB_Design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Nguyen-Dinh-Si-Khoa\Learn-NodeJS\2-How-Node-Works\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CFEEB6CB-3A62-4781-B70A-730C22F0C6E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3194917B-DFC2-410C-A145-CF26A3F0AF94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B37F2202-0D3B-4A9E-ADDA-AE3FE7470749}"/>
   </bookViews>
@@ -140,7 +140,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -160,6 +160,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -200,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -208,10 +216,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
@@ -1428,8 +1437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8069AFA4-3071-47A2-898A-D241D6032415}">
   <dimension ref="B2:P20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1454,7 +1463,7 @@
       <c r="K2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="6"/>
+      <c r="L2" s="5"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D3" s="2" t="s">
@@ -1463,22 +1472,22 @@
       <c r="F3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="8" t="s">
         <v>5</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="K3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="7"/>
+      <c r="L3" s="6"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="8" t="s">
         <v>1</v>
       </c>
       <c r="G4" s="4" t="s">
@@ -1487,7 +1496,7 @@
       <c r="K4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="8"/>
+      <c r="L4" s="7"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D5" s="4" t="s">
@@ -1499,16 +1508,16 @@
       <c r="J5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="K5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="L5" s="8"/>
+      <c r="L5" s="7"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="F6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="9" t="s">
         <v>1</v>
       </c>
       <c r="M6" s="2" t="s">
@@ -1516,7 +1525,7 @@
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="M7" s="3" t="s">
+      <c r="M7" s="8" t="s">
         <v>23</v>
       </c>
       <c r="N7" t="s">
@@ -1527,7 +1536,7 @@
       <c r="C8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M8" s="3" t="s">
+      <c r="M8" s="8" t="s">
         <v>10</v>
       </c>
       <c r="N8" t="s">
@@ -1538,7 +1547,7 @@
       <c r="B9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="8" t="s">
         <v>13</v>
       </c>
       <c r="I9" s="2" t="s">
@@ -1552,7 +1561,7 @@
       <c r="C10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="I10" s="8" t="s">
         <v>18</v>
       </c>
       <c r="M10" s="4" t="s">
@@ -1563,7 +1572,7 @@
       <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>5</v>
       </c>
       <c r="I11" s="4" t="s">
@@ -1574,7 +1583,7 @@
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="O12" s="3" t="s">
+      <c r="O12" s="8" t="s">
         <v>23</v>
       </c>
       <c r="P12" t="s">
@@ -1593,7 +1602,7 @@
       <c r="C14" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="G14" s="8" t="s">
         <v>16</v>
       </c>
       <c r="O14" s="4" t="s">
@@ -1604,13 +1613,13 @@
       <c r="B15" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="8" t="s">
         <v>16</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="O15" s="4" t="s">
+      <c r="O15" s="3" t="s">
         <v>26</v>
       </c>
       <c r="P15" t="s">
@@ -1621,17 +1630,17 @@
       <c r="B16" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="8" t="s">
         <v>5</v>
       </c>
       <c r="F16" s="1"/>
-      <c r="G16" s="4" t="s">
+      <c r="G16" s="3" t="s">
         <v>5</v>
       </c>
       <c r="H16" t="s">
         <v>8</v>
       </c>
-      <c r="O16" s="5" t="s">
+      <c r="O16" s="9" t="s">
         <v>30</v>
       </c>
       <c r="P16" t="s">
@@ -1642,10 +1651,10 @@
       <c r="B17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="G17" s="3" t="s">
         <v>13</v>
       </c>
       <c r="H17" t="s">
@@ -1653,7 +1662,7 @@
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="G18" s="4" t="s">
+      <c r="G18" s="3" t="s">
         <v>18</v>
       </c>
       <c r="H18" t="s">
@@ -1672,13 +1681,13 @@
       <c r="D20" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="8" t="s">
         <v>16</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J20" s="3" t="s">
+      <c r="J20" s="8" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>